<commit_message>
Costed Level 1 units.
</commit_message>
<xml_diff>
--- a/Streak 3/New Units.xlsx
+++ b/Streak 3/New Units.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="New Units" sheetId="1" r:id="rId1"/>
     <sheet name="Upgrades" sheetId="2" r:id="rId2"/>
     <sheet name="Promotions" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
   <si>
     <r>
       <t xml:space="preserve">Unit strength increases +15% per tier for </t>
@@ -89,9 +90,6 @@
     <t>Golem (ALL)</t>
   </si>
   <si>
-    <t>Lesser Golem 87 (-15%)</t>
-  </si>
-  <si>
     <t>Golem 115 (-15%)</t>
   </si>
   <si>
@@ -99,10 +97,6 @@
   </si>
   <si>
     <t>Assault (1)</t>
-  </si>
-  <si>
-    <t>Axeman 100
-15% Vs Company</t>
   </si>
   <si>
     <t>Swordsman 132
@@ -116,10 +110,6 @@
     <t>Ranged (2)</t>
   </si>
   <si>
-    <t>Archer 100
-15% Vs Assault</t>
-  </si>
-  <si>
     <t>Longbowman 132
 15% Vs Assault</t>
   </si>
@@ -131,10 +121,6 @@
     <t>Company (3)</t>
   </si>
   <si>
-    <t>Militia 100
-15% Vs Ranged</t>
-  </si>
-  <si>
     <t>Spearman 132
 15% Vs Ranged</t>
   </si>
@@ -144,14 +130,6 @@
   </si>
   <si>
     <t>Melee</t>
-  </si>
-  <si>
-    <t>Warrior 76</t>
-  </si>
-  <si>
-    <t>Bandit 91
-Pillage x2
-15% Forest/Jungle Strength</t>
   </si>
   <si>
     <t>Highlander 120
@@ -164,12 +142,6 @@
   </si>
   <si>
     <t>Mounted (4)</t>
-  </si>
-  <si>
-    <t>Horseman 95 (-5%)
-2 Moves
-10% Withdraw
-No Def Bonus</t>
   </si>
   <si>
     <t>Knight 126 (-5%)
@@ -188,12 +160,6 @@
     <t>Elephant (4)</t>
   </si>
   <si>
-    <t>Elephant 120 – Limit 3
-2 Moves
-Uses 2 Stack Capacity
-No Def Bonus</t>
-  </si>
-  <si>
     <t>War Elephant 158 – Limit 3
 2 Moves
 Uses 2 Stack Capacity
@@ -203,25 +169,11 @@
     <t>Recon (5)</t>
   </si>
   <si>
-    <t>Scout 46
-2 Moves
-Ignore Terrain Cost</t>
-  </si>
-  <si>
-    <t>Hunter 91 (-10%)
-See Invis
-Carry Hawk</t>
-  </si>
-  <si>
     <t>Hawk
 3x3 area</t>
   </si>
   <si>
     <t>Ranger</t>
-  </si>
-  <si>
-    <t>Ranger 91
-Move Impassable Terrain</t>
   </si>
   <si>
     <t>Forester 120
@@ -232,9 +184,6 @@
     <t>Arcane (6)</t>
   </si>
   <si>
-    <t>Adept 76</t>
-  </si>
-  <si>
     <t>Mage 91</t>
   </si>
   <si>
@@ -246,11 +195,6 @@
   </si>
   <si>
     <t>Beast (7)</t>
-  </si>
-  <si>
-    <t>Drown 95
-Water Walking
-No Happy</t>
   </si>
   <si>
     <t>Stygian Drown 126
@@ -275,13 +219,6 @@
     <t>Navy</t>
   </si>
   <si>
-    <t>Galley 91
-Capacity: 2
-Ocean Def Bonus?
-No Ocean
-No Happy</t>
-  </si>
-  <si>
     <t>Caravel 120
 Capacity: 3
 Sentry 1
@@ -295,13 +232,6 @@
 Ocean Def Bonus?
 Bombard 10%
 No Happy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trireme 100
-Ocean Def Bonus?
-No Ocean
-No Happy
-</t>
   </si>
   <si>
     <t>Galleon 132
@@ -349,15 +279,6 @@
 No Pillage</t>
   </si>
   <si>
-    <t xml:space="preserve">Myconid 46
-Cast Bloom (3 turns)
-Can't attack
-No Happy
-No Defence
-No Pillage
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dwarf 46
 Can Uplift (4 turns)
 Can't attack
@@ -387,13 +308,6 @@
 No Happy</t>
   </si>
   <si>
-    <t>Baby Spider 91
-Invisible
-No Def
-No Pillage
-No Happy</t>
-  </si>
-  <si>
     <t>Drown Hunting Pack 167
 Water Walking
 No Happy</t>
@@ -419,13 +333,6 @@
 No Def
 No Pillage
 No Happy</t>
-  </si>
-  <si>
-    <t>Battering Ram 10
-Bombard 10%
-No Attack
-No Upkeep
-Not Alive</t>
   </si>
   <si>
     <t>Catapult 30
@@ -631,6 +538,138 @@
   <si>
     <t>Invisibility Boots
 Imperial</t>
+  </si>
+  <si>
+    <t>Warrior 76
+20H</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Hammers</t>
+  </si>
+  <si>
+    <t>Militia</t>
+  </si>
+  <si>
+    <t>Str/Hammers</t>
+  </si>
+  <si>
+    <t>Axeman</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Scout 46
+2 Moves
+Ignore Terrain Cost
+20H</t>
+  </si>
+  <si>
+    <t>Axeman 100
+15% Vs Company
+60H</t>
+  </si>
+  <si>
+    <t>Archer 100
+15% Vs Assault
+60H</t>
+  </si>
+  <si>
+    <t>Militia 100
+15% Vs Ranged
+60H</t>
+  </si>
+  <si>
+    <t>Horseman 95 (-5%)
+2 Moves
+10% Withdraw
+No Def Bonus
+60H</t>
+  </si>
+  <si>
+    <t>Hunter 91 (-10%)
+See Invis
+Carry Hawk
+50H</t>
+  </si>
+  <si>
+    <t>Lesser Golem 87 (-15%)
+34H</t>
+  </si>
+  <si>
+    <t>Bandit 91
+Pillage x2
+15% Forest/Jungle Strength
+48H</t>
+  </si>
+  <si>
+    <t>50H</t>
+  </si>
+  <si>
+    <t>Ranger 91
+Move Impassable Terrain
+45H</t>
+  </si>
+  <si>
+    <t>Adept 76
+75H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myconid 46
+Cast Bloom (4 turns)
+Double Move Forest/Jungle
+No Happy
+No Pillage
+25H
+</t>
+  </si>
+  <si>
+    <t>Baby Spider 91
+Invisible
+No Def
+No Pillage
+No Happy
+48H</t>
+  </si>
+  <si>
+    <t>Drown 95
+Water Walking
+No Happy
+55H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trireme 100
+Ocean Def Bonus?
+No Ocean
+No Happy
+60H
+</t>
+  </si>
+  <si>
+    <t>Galley 91
+Capacity: 2
+Ocean Def Bonus?
+No Ocean
+No Happy
+48H</t>
+  </si>
+  <si>
+    <t>Battering Ram 10
+Bombard 10%
+No Attack
+No Upkeep
+Not Alive
+20H</t>
+  </si>
+  <si>
+    <t>Elephant 120 – Limit 3
+2 Moves
+Uses 2 Stack Capacity
+No Def Bonus
+108H</t>
   </si>
 </sst>
 </file>
@@ -755,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -882,6 +921,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1338,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1433,71 +1475,71 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
+      <c r="D6" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1505,20 +1547,20 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="16" t="s">
-        <v>25</v>
+      <c r="C14" s="44" t="s">
+        <v>109</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1528,7 +1570,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="35"/>
@@ -1539,16 +1581,16 @@
     </row>
     <row r="17" spans="1:9" s="18" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1563,7 +1605,7 @@
       <c r="D19" s="19"/>
       <c r="F19" s="19"/>
       <c r="H19" s="39" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="I19" s="19"/>
     </row>
@@ -1605,15 +1647,15 @@
     <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
     </row>
-    <row r="26" spans="1:9" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="18" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1621,17 +1663,17 @@
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="C28"/>
       <c r="D28" s="9" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="I28" s="9"/>
     </row>
@@ -1640,7 +1682,7 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H29" s="36"/>
     </row>
@@ -1648,7 +1690,9 @@
       <c r="A30" s="22"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="H30" s="36"/>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1670,16 +1714,16 @@
     </row>
     <row r="34" spans="1:9" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1715,19 +1759,19 @@
     </row>
     <row r="40" spans="1:9" s="26" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>126</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
@@ -1736,24 +1780,24 @@
     <row r="42" spans="1:9" s="26" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A42" s="25"/>
       <c r="D42" s="37" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="26" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A43" s="25"/>
       <c r="D43" s="37"/>
       <c r="F43" s="27" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="26" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A44" s="25"/>
       <c r="D44" s="37"/>
       <c r="F44" s="27" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
@@ -1771,148 +1815,136 @@
     </row>
     <row r="48" spans="1:9" s="29" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="H48" s="38" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="I48" s="38"/>
     </row>
     <row r="49" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="31"/>
     </row>
-    <row r="50" spans="1:9" s="29" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="29" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="28"/>
       <c r="D50" s="30" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" s="29" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="H52" s="38" t="s">
-        <v>77</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="28"/>
+      <c r="D51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="H51" s="30"/>
+    </row>
+    <row r="52" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="28"/>
+      <c r="D52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="H52" s="30"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:9" s="33" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F54" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="H54" s="40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
-    </row>
-    <row r="56" spans="1:9" s="33" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="29" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" s="33" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="F56" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="H56" s="34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="33" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="H56" s="40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="32"/>
-      <c r="E57" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G57" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I57" s="34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="32"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>62</v>
-      </c>
+    </row>
+    <row r="58" spans="1:9" s="33" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H58" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="33" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="32"/>
+      <c r="E59" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="I59" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="32"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
+      <c r="A64" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-      <c r="J65"/>
+      <c r="A65" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-      <c r="J66"/>
+      <c r="A66" s="3"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67"/>
@@ -2321,6 +2353,30 @@
       <c r="H100"/>
       <c r="I100"/>
       <c r="J100"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2337,7 +2393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2353,44 +2409,44 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="42" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -2406,19 +2462,19 @@
     </row>
     <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2430,19 +2486,19 @@
     </row>
     <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>120</v>
-      </c>
       <c r="D8" s="43" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2453,19 +2509,19 @@
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>121</v>
-      </c>
       <c r="D10" s="43" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2477,19 +2533,19 @@
     </row>
     <row r="12" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>122</v>
-      </c>
       <c r="D12" s="43" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2501,13 +2557,13 @@
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="43" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E14" s="43"/>
     </row>
@@ -2520,13 +2576,13 @@
     <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="41" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E16" s="43"/>
     </row>
@@ -2538,7 +2594,7 @@
     </row>
     <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B18" s="41" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C18" s="43"/>
     </row>
@@ -2576,7 +2632,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A4:C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2588,20 +2644,20 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2613,7 +2669,7 @@
     </row>
     <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2625,7 +2681,7 @@
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -2637,7 +2693,7 @@
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -2649,7 +2705,7 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -2661,7 +2717,7 @@
     </row>
     <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -2674,4 +2730,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="0">B3/C3</f>
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>